<commit_message>
casos de uso actualizados con descripciones (algunos)
</commit_message>
<xml_diff>
--- a/PlanDeProyecto/Anexos.xlsx
+++ b/PlanDeProyecto/Anexos.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="91">
   <si>
     <t>Proyecto</t>
   </si>
@@ -80,12 +80,6 @@
     <t>RF4</t>
   </si>
   <si>
-    <t>&lt;Requerimiento Funcional Nº5&gt;</t>
-  </si>
-  <si>
-    <t>RF5</t>
-  </si>
-  <si>
     <t>&lt;Requerimiento Funcional Distintivo&gt;</t>
   </si>
   <si>
@@ -176,9 +170,6 @@
     <t>Ver Estadísticas</t>
   </si>
   <si>
-    <t>Hambre, cansancio, Stamina, Felicidad</t>
-  </si>
-  <si>
     <t>Ir al baño</t>
   </si>
   <si>
@@ -267,19 +258,81 @@
   </si>
   <si>
     <t>RFD-RF4</t>
+  </si>
+  <si>
+    <t>Requerimientos</t>
+  </si>
+  <si>
+    <t>Casos de uso</t>
+  </si>
+  <si>
+    <t>Casos de Uso</t>
+  </si>
+  <si>
+    <t>Dirigir al robot a través del celular</t>
+  </si>
+  <si>
+    <t>Robot camina de acuerdo a instrucciones dadas</t>
+  </si>
+  <si>
+    <t>Adecuar al robot para distintas condiciones ambiantales (luz,sonido,etc)</t>
+  </si>
+  <si>
+    <t>Da instrucciones a la mascota para que vaya a dormir</t>
+  </si>
+  <si>
+    <t>Robot recoge una pelota del suelo</t>
+  </si>
+  <si>
+    <t>Dar alimentos a mascota virtual</t>
+  </si>
+  <si>
+    <t>Robot come</t>
+  </si>
+  <si>
+    <t>Robot duerme</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -296,7 +349,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -332,11 +385,80 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -345,9 +467,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -361,15 +480,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -393,23 +503,271 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="3"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="3" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Título 1" xfId="1" builtinId="16"/>
+    <cellStyle name="Título 2" xfId="2" builtinId="17"/>
+    <cellStyle name="Título 3" xfId="3" builtinId="18"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="9">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top style="thick">
+          <color auto="1"/>
+        </top>
+        <bottom style="thick">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top style="thick">
+          <color auto="1"/>
+        </top>
+        <bottom style="thick">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top style="thick">
+          <color auto="1"/>
+        </top>
+        <bottom style="thick">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -485,6 +843,84 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A4:D13" totalsRowShown="0">
+  <autoFilter ref="A4:D13"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Requerimientos" dataDxfId="8"/>
+    <tableColumn id="2" name="Abr." dataDxfId="7"/>
+    <tableColumn id="3" name="Descripción"/>
+    <tableColumn id="4" name="Observaciones" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla3" displayName="Tabla3" ref="A25:D44" totalsRowShown="0">
+  <autoFilter ref="A25:D44"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Casos de uso" dataDxfId="5"/>
+    <tableColumn id="2" name="Ref." dataDxfId="4"/>
+    <tableColumn id="3" name="Descripción" dataDxfId="3"/>
+    <tableColumn id="4" name="Nº Entregable" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla4" displayName="Tabla4" ref="B3:E8" totalsRowShown="0">
+  <autoFilter ref="B3:E8"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Casos de uso"/>
+    <tableColumn id="2" name="Ref"/>
+    <tableColumn id="3" name="Descripción"/>
+    <tableColumn id="4" name="% Cumplimiento"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla5" displayName="Tabla5" ref="B3:E10" totalsRowShown="0">
+  <autoFilter ref="B3:E10"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Casos de Uso"/>
+    <tableColumn id="2" name="Ref" dataDxfId="1"/>
+    <tableColumn id="3" name="Descripción"/>
+    <tableColumn id="4" name="% Cumplimiento"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla6" displayName="Tabla6" ref="B3:E8" totalsRowShown="0">
+  <autoFilter ref="B3:E8"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Casos de Uso"/>
+    <tableColumn id="2" name="Ref" dataDxfId="0"/>
+    <tableColumn id="3" name="Descripción"/>
+    <tableColumn id="4" name="% Cumplimiento"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla7" displayName="Tabla7" ref="B3:E5" totalsRowShown="0">
+  <autoFilter ref="B3:E5"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Casos de Uso"/>
+    <tableColumn id="2" name="Ref"/>
+    <tableColumn id="3" name="Descripción"/>
+    <tableColumn id="4" name="% Cumplimiento"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -776,523 +1212,557 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.85546875"/>
-    <col min="2" max="2" width="7" style="1" customWidth="1"/>
-    <col min="3" max="3" width="78.140625"/>
+    <col min="2" max="2" width="8" style="1" customWidth="1"/>
+    <col min="3" max="3" width="83.85546875" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" style="1"/>
     <col min="5" max="5" width="20.28515625"/>
     <col min="6" max="1025" width="10.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3"/>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:5" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="23"/>
+      <c r="C2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="5"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" ht="34.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" t="s">
+      <c r="B3" s="26"/>
+      <c r="C3" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="5"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
-        <v>74</v>
-      </c>
-      <c r="D6" s="12"/>
+      <c r="C6" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="31"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="31"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="31"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="12"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>71</v>
-      </c>
-      <c r="D8" s="12"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D9" s="12"/>
+      <c r="D9" s="31"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="12"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="C10" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="31"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="11" t="s">
+    </row>
+    <row r="12" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D11" s="12" t="s">
+      <c r="B12" s="33" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="8" t="s">
+      <c r="C12" s="30"/>
+      <c r="D12" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="12"/>
+    <row r="13" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="39"/>
+      <c r="B13" s="40"/>
+      <c r="D13" s="31"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14"/>
       <c r="D14"/>
     </row>
     <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="8" t="s">
+      <c r="A17" s="9"/>
+      <c r="B17" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="E17" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="C18" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="7"/>
+    </row>
+    <row r="19" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="8" t="s">
+      <c r="B19" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="8"/>
-    </row>
-    <row r="19" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="D19" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C20" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="8">
+      <c r="D20" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="8" t="s">
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="8">
+      <c r="C23" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="13"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="14"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="D28" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="D30" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="30"/>
+      <c r="D31" s="35">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" s="8" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" s="30"/>
+      <c r="D32" s="36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" s="30"/>
+      <c r="D33" s="36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="D34" s="36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" s="8">
+      <c r="C35" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="D35" s="36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="B36" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C36" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="D36" s="36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="D37" s="36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="D38" s="35">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D22" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="8" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="C39" s="30"/>
+      <c r="D39" s="35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="C40" s="30"/>
+      <c r="D40" s="35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C41" s="30"/>
+      <c r="D41" s="36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B42" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D23" s="8">
+      <c r="C42" s="30"/>
+      <c r="D42" s="36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="B43" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" s="30"/>
+      <c r="D43" s="35">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="18"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="20"/>
-      <c r="B25" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" s="20" t="s">
+    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="B44" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C44" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D44" s="36">
         <v>4</v>
       </c>
-      <c r="D25" s="21" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>44</v>
-      </c>
-      <c r="B26" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="D26" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>46</v>
-      </c>
-      <c r="B27" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C27" t="s">
-        <v>47</v>
-      </c>
-      <c r="D27" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>75</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D28" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>55</v>
-      </c>
-      <c r="B29" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D29" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>57</v>
-      </c>
-      <c r="B30" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="D30" s="25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>58</v>
-      </c>
-      <c r="B31" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="D31" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>51</v>
-      </c>
-      <c r="B32" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32" t="s">
-        <v>52</v>
-      </c>
-      <c r="D32" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>77</v>
-      </c>
-      <c r="B33" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="D33" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>49</v>
-      </c>
-      <c r="B34" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="D34" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>54</v>
-      </c>
-      <c r="B35" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D35" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>78</v>
-      </c>
-      <c r="B36" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="D36" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>56</v>
-      </c>
-      <c r="B37" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D37" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>79</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D38" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>80</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D39" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>81</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D40" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>48</v>
-      </c>
-      <c r="B41" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="D41" s="23">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>53</v>
-      </c>
-      <c r="B42" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D42" s="23">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>59</v>
-      </c>
-      <c r="B43" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D43" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>73</v>
-      </c>
-      <c r="B44" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="C44" t="s">
-        <v>50</v>
-      </c>
-      <c r="D44" s="23">
-        <v>4</v>
-      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B45" s="21"/>
-      <c r="D45" s="23"/>
+      <c r="B45" s="17"/>
+      <c r="D45" s="18"/>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" s="24"/>
+      <c r="B49" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1301,7 +1771,7 @@
   <dimension ref="B3:E8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C8"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1310,79 +1780,85 @@
     <col min="2" max="2" width="28.7109375"/>
     <col min="3" max="3" width="7.5703125" customWidth="1"/>
     <col min="4" max="4" width="37.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
     <col min="6" max="1025" width="10.7109375"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>81</v>
+      </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
       </c>
       <c r="E3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="15" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="19" t="s">
+      <c r="C6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="19" t="s">
+      <c r="C7" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>33</v>
+      <c r="C8" s="19" t="s">
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1391,7 +1867,7 @@
   <dimension ref="B3:E11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1400,105 +1876,111 @@
     <col min="2" max="2" width="28.7109375"/>
     <col min="3" max="3" width="10.42578125" customWidth="1"/>
     <col min="4" max="4" width="32.140625"/>
-    <col min="5" max="5" width="15.42578125"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
     <col min="6" max="1025" width="10.7109375"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
       </c>
       <c r="E3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="15" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="19" t="s">
+      <c r="C6" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="19" t="s">
+      <c r="C7" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="C8" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="19" t="s">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B7" s="19" t="s">
+      <c r="C9" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="C7" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="D7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" s="24" t="s">
+      <c r="C10" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B9" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="D9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>13</v>
-      </c>
       <c r="D10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="19"/>
-      <c r="C11" s="23"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1507,7 +1989,7 @@
   <dimension ref="B3:E8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1516,81 +1998,87 @@
     <col min="2" max="2" width="15"/>
     <col min="3" max="3" width="11.5703125"/>
     <col min="4" max="4" width="25.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
     <col min="6" max="6" width="10.7109375"/>
     <col min="7" max="7" width="11.5703125"/>
     <col min="8" max="1025" width="10.7109375"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="19" t="s">
-        <v>62</v>
+      <c r="B4" s="15" t="s">
+        <v>59</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="19" t="s">
-        <v>63</v>
+      <c r="B5" s="15" t="s">
+        <v>60</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="19" t="s">
-        <v>64</v>
+      <c r="B6" s="15" t="s">
+        <v>61</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>76</v>
+      <c r="B7" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>73</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" s="24" t="s">
+      <c r="B8" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="19" t="s">
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1599,7 +2087,7 @@
   <dimension ref="B3:E6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1608,50 +2096,56 @@
     <col min="2" max="2" width="28.7109375"/>
     <col min="3" max="3" width="10" customWidth="1"/>
     <col min="4" max="4" width="17.7109375"/>
-    <col min="5" max="5" width="15.42578125"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
     <col min="6" max="6" width="10.7109375"/>
     <col min="7" max="7" width="11.5703125"/>
     <col min="8" max="1025" width="10.7109375"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" s="24" t="s">
+      <c r="B4" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="19" t="s">
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>82</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>79</v>
       </c>
       <c r="D5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C6" s="21"/>
+      <c r="C6" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>